<commit_message>
Added raw CSVs, looked at layoffs by IPO status
Added raw CSVs to repo.
Looked at number of companies with layoffs by IPO status.
</commit_message>
<xml_diff>
--- a/tech_layoffs_research/exports/tech_layoffs_results.xlsx
+++ b/tech_layoffs_research/exports/tech_layoffs_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbryant/Documents/GitHub/SQL_Projects/tech_layoffs_research/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BC543D-E813-6543-B024-CF8B88B7FA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B4D75F-EFF6-9846-841E-73D7CEBEA968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{D5FE2044-42E5-F445-8EAD-A3BDB9DA7242}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{D5FE2044-42E5-F445-8EAD-A3BDB9DA7242}"/>
   </bookViews>
   <sheets>
     <sheet name="layoffs_by_city" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="avg_percent_impacted_by_city" sheetId="3" r:id="rId3"/>
     <sheet name="layoffs_by_quarter" sheetId="4" r:id="rId4"/>
     <sheet name="comp_layoffs_interestRates" sheetId="5" r:id="rId5"/>
+    <sheet name="layoffs_by_IPOstatus" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Seattle</t>
   </si>
@@ -133,6 +134,21 @@
   </si>
   <si>
     <t>monthly_layoffs</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>num_companies</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>LAYOFFS BY IPO STATUS</t>
   </si>
 </sst>
 </file>
@@ -4263,7 +4279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EA780F-C220-8944-BCAF-819AA7D7B6E4}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" workbookViewId="0">
+    <sheetView zoomScale="190" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -4566,4 +4582,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DEAB901-DE36-DF40-8BD5-2B8A2ADA5737}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>